<commit_message>
Added parts (fotos and STL-files)
</commit_message>
<xml_diff>
--- a/Hardware/Bill of Materials.xlsx
+++ b/Hardware/Bill of Materials.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/berend/Documents/GitHub/Tekenrobot/Hardware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9319B5E4-BE61-4145-B266-875D338A0A27}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD2E5A0-FF27-FC49-88AB-DA9395E6A2A3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="17540" xr2:uid="{5917031B-F97C-174E-B176-4156F98790EC}"/>
+    <workbookView xWindow="4600" yWindow="3760" windowWidth="14400" windowHeight="17540" xr2:uid="{5917031B-F97C-174E-B176-4156F98790EC}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
   <si>
     <t>Description</t>
   </si>
@@ -42,18 +42,12 @@
     <t>Qty</t>
   </si>
   <si>
-    <t>Where to get it</t>
-  </si>
-  <si>
     <t>Robot body</t>
   </si>
   <si>
     <t>Printed part</t>
   </si>
   <si>
-    <t>Wheels</t>
-  </si>
-  <si>
     <t>Guiderail</t>
   </si>
   <si>
@@ -84,18 +78,6 @@
     <t>4-lead female-female jumper wire</t>
   </si>
   <si>
-    <t>Hobby servo all-metal 9g</t>
-  </si>
-  <si>
-    <t>O-ring 3.5mm x 38mm</t>
-  </si>
-  <si>
-    <t>philips screw 2.9mm x 16 mm</t>
-  </si>
-  <si>
-    <t>philips screw 2.9mm x 6.5 mm</t>
-  </si>
-  <si>
     <t>Bearing Ball 9mm</t>
   </si>
   <si>
@@ -114,21 +96,83 @@
     <t>Voltage regulator ultra-low drop TS2940</t>
   </si>
   <si>
-    <t>jumper header 4x1 pin</t>
-  </si>
-  <si>
     <t>Ferrule 0.25mm2 x 6mm (isolated)</t>
   </si>
   <si>
     <t>Dome (half of transparent decorative ball) 60mm</t>
+  </si>
+  <si>
+    <t>Right Wheel</t>
+  </si>
+  <si>
+    <t>Left Wheel</t>
+  </si>
+  <si>
+    <t>hema.nl</t>
+  </si>
+  <si>
+    <t>O-ring 3.1mm x 37mm</t>
+  </si>
+  <si>
+    <t>Bluetooth module (HC-05 or JDY-30)</t>
+  </si>
+  <si>
+    <t>Hobby servo metal-gear 9g</t>
+  </si>
+  <si>
+    <t>raised head philips screw 2.9mm x 6.5 mm</t>
+  </si>
+  <si>
+    <t>raised head philips screw 2.9mm x 16 mm</t>
+  </si>
+  <si>
+    <t>pin strip, straight 4x1 pin</t>
+  </si>
+  <si>
+    <t>included with Arduino</t>
+  </si>
+  <si>
+    <t>Est. Cost</t>
+  </si>
+  <si>
+    <t>Est. Cost per item</t>
+  </si>
+  <si>
+    <t>any hobby shop</t>
+  </si>
+  <si>
+    <t>DIY shop</t>
+  </si>
+  <si>
+    <t>AliExpress</t>
+  </si>
+  <si>
+    <t>Local electronics store</t>
+  </si>
+  <si>
+    <t>Where I got it</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -156,8 +200,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,329 +519,613 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56A749A3-230E-C747-B506-CEE7B3E4560C}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="42" customWidth="1"/>
-    <col min="4" max="4" width="26.83203125" customWidth="1"/>
+    <col min="4" max="5" width="10.83203125" style="1"/>
+    <col min="6" max="6" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>4.43</v>
+      </c>
+      <c r="E2" s="1">
+        <f>D2*C2</f>
+        <v>4.43</v>
+      </c>
+      <c r="F2" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.09</v>
+      </c>
+      <c r="E3" s="1">
+        <f t="shared" ref="E3:E28" si="0">D3*C3</f>
+        <v>0.09</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D4" s="1">
+        <v>0.09</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" si="0"/>
+        <v>0.09</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D5" s="1">
+        <v>0.11</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="0"/>
+        <v>0.11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D6" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.21</v>
+      </c>
+      <c r="F6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D7" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="F7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
-      <c r="D8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D8" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="0"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C9">
-        <v>2</v>
-      </c>
-      <c r="D9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="F9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="C10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="F10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D11" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="F11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D12" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" si="0"/>
+        <v>0.05</v>
+      </c>
+      <c r="F12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1.22</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="0"/>
+        <v>2.44</v>
+      </c>
+      <c r="F14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D15" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
+      <c r="F15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16" s="1">
+        <v>1.77</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="0"/>
+        <v>1.77</v>
+      </c>
+      <c r="F16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17" s="1">
+        <v>2.12</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="0"/>
+        <v>2.12</v>
+      </c>
+      <c r="F17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="0"/>
+        <v>0.95</v>
+      </c>
+      <c r="F18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C19">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4</v>
+      </c>
+      <c r="F19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="0"/>
+        <v>0.24</v>
+      </c>
+      <c r="F20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="D21" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="0"/>
+        <v>0.42000000000000004</v>
+      </c>
+      <c r="F21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="D22" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="0"/>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C23">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="0"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="E24" s="1">
+        <f t="shared" si="0"/>
+        <v>0.24</v>
+      </c>
+      <c r="F24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="E25" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E26" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="F26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28">
         <v>12</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="E28" s="1">
+        <f t="shared" si="0"/>
+        <v>0.48</v>
+      </c>
+      <c r="F28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D29" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" s="2">
+        <f>SUM(E2:E28)</f>
+        <v>23.15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>